<commit_message>
fixed bugs for sp
</commit_message>
<xml_diff>
--- a/m1/js/doc/CreatePanelsControl.xlsx
+++ b/m1/js/doc/CreatePanelsControl.xlsx
@@ -9,12 +9,12 @@
   </bookViews>
   <sheets>
     <sheet name="state-chart" sheetId="1" r:id="rId1"/>
-    <sheet name="itemsinfo" sheetId="1380" r:id="rId1387"/>
-    <sheet name="help" sheetId="1379" r:id="rId1386"/>
-    <sheet name="setting.ini" sheetId="1378" r:id="rId1385"/>
-    <sheet name="template-statefunc" sheetId="1377" r:id="rId1384"/>
-    <sheet name="template-source" sheetId="1376" r:id="rId1383"/>
-    <sheet name="config" sheetId="1375" r:id="rId1382"/>
+    <sheet name="itemsinfo" sheetId="1386" r:id="rId1393"/>
+    <sheet name="help" sheetId="1385" r:id="rId1392"/>
+    <sheet name="setting.ini" sheetId="1384" r:id="rId1391"/>
+    <sheet name="template-statefunc" sheetId="1383" r:id="rId1390"/>
+    <sheet name="template-source" sheetId="1382" r:id="rId1389"/>
+    <sheet name="config" sheetId="1381" r:id="rId1388"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3549" uniqueCount="788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3556" uniqueCount="790">
   <si>
     <t>state</t>
     <phoneticPr fontId="2"/>
@@ -22395,6 +22395,93 @@
   </si>
   <si>
     <t>; The setting was created automatically. 2019/04/08 21:42:13
+; * pssgEditor version : 0.23.40293.f0b9fd4248d354ec440680d9161406ae26d4945e
+psggfile=@@@
+CreatePanelsControl.psgg
+@@@
+xlsfile=@@@
+CreatePanelsControl.xlsx
+@@@
+guid=@@@
+a7e00d9d-8650-4495-a1cb-7e88de8b22e1
+@@@
+bitmap_width=5000
+bitmap_height=2000
+c_statec_cmt=1
+c_thumbnail=1
+c_contents=1
+force_display_outpin=0
+last_action=@@@
+Edited a state.
+@@@
+target_pathdir=@@@
+/
+@@@
+state_location_list=@@@
+@@@
+nodegroup_comment_list=@@@
+[{"Key":"\/","Value":"This is the root"}]
+@@@
+nodegroup_pos_list=@@@
+[{"Key":"\/","Value":{"x":100,"y":100}}]
+@@@
+fillter_state_location_list=@@@
+[{"Key":"\/","Value":[{"Key":"S_START","Value":{"x":22,"y":15}},{"Key":"S_END","Value":{"x":2346,"y":519}},{"Key":"S_CREATE_BUTTON1","Value":{"x":2486,"y":199}},{"Key":"S_SET_DATA","Value":{"x":915,"y":204}},{"Key":"S_FORINIT","Value":{"x":1155,"y":90}},{"Key":"S_FORNEXT","Value":{"x":1094,"y":647}},{"Key":"S_GET_ITEM","Value":{"x":1155,"y":247}},{"Key":"S_WAIT_REQ","Value":{"x":82,"y":221}},{"Key":"S_WAIT_REQ1","Value":{"x":225,"y":27}},{"Key":"S_CB","Value":{"x":2229,"y":679}},{"Key":"S_CREATE_PANELS","Value":{"x":1550,"y":239}},{"Key":"S_LOAD_TEXTUREX","Value":{"x":2307,"y":192}},{"Key":"S_LOADTEX","Value":{"x":1343,"y":240}},{"Key":"S_LOAD_BBTEX","Value":{"x":1790,"y":679}},{"Key":"S_CREATE_BACKBOARD","Value":{"x":2022,"y":687}},{"Key":"S_SET_MAPINFO","Value":{"x":1981,"y":245}},{"Key":"S_LOAD_TOCHTEX","Value":{"x":553,"y":193}},{"Key":"S_VAR_TOUCHTEX","Value":{"x":350,"y":219}},{"Key":"S_CREATE_TOUCHCOL","Value":{"x":1755,"y":235}}]}]
+@@@
+linecolor_data=@@@
+[{"color":{"knownColor":0,"name":null,"state":2,"value":4285493103},"pattern":"BACKTO_"}]
+@@@
+use_external_command=0
+external_command=@@@
+@@@
+source_editor=@@@
+"C:\Program Files (x86)\Brackets\Brackets.exe" %1
+@@@
+source_editor_vs2015_support=1
+label_show=0
+label_text=@@@
+test
+@@@
+option_delete_thisstring=0
+option_delete_br_string=1
+option_delete_bracket_string=1
+option_delete_s_state_string=1
+option_copy_output_to_clipboard=0
+option_convert_with_confirm=0
+option_omit_basestate_string=0
+option_hide_basestate_contents=1
+option_hide_branchcmt_onbranchbox=0
+font_name=@@@
+MS UI Gothic
+@@@
+font_size=11
+comment_font_size=0
+contents_font_size=0
+state_width=140
+state_height=20
+comment_block_height=4
+content_max_height=200
+comment_block_fixed=0
+line_space=-1
+userbutton_title=@@@
+@@@
+userbutton_command=@@@
+@@@
+userbutton_callafterconvert=0
+</t>
+  </si>
+  <si>
+    <t>this.box = new THREE.Mesh(
+    new THREE.PlaneGeometry(512, 512),
+    new THREE.MeshBasicMaterial({map: this.texture})  // {map: texture}がキモ
+);
+this.box.position.set(0,0,-2);
+this.box.name = "backboard";
+G.scene.add(this.box);
+</t>
+  </si>
+  <si>
+    <t>; The setting was created automatically. 2019/04/13 19:59:15
 ; * pssgEditor version : 0.23.40293.f0b9fd4248d354ec440680d9161406ae26d4945e
 psggfile=@@@
 CreatePanelsControl.psgg
@@ -23675,7 +23762,7 @@
         <v>355</v>
       </c>
       <c r="R13" s="10" t="s">
-        <v>772</v>
+        <v>788</v>
       </c>
       <c r="S13" s="10" t="s">
         <v>774</v>
@@ -24805,21 +24892,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet1375.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet1381.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>787</v>
+        <v>789</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet1376.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet1382.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -24833,7 +24920,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet1377.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet1383.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -24847,7 +24934,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet1378.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet1384.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -24861,7 +24948,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet1379.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet1385.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -24875,7 +24962,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet1380.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet1386.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>